<commit_message>
Add normalization excel file
</commit_message>
<xml_diff>
--- a/_docs/trim03/03_Database_sql/03_Normalizacion/Normalizacion db-tracklinker.xlsx
+++ b/_docs/trim03/03_Database_sql/03_Normalizacion/Normalizacion db-tracklinker.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
   <si>
     <r>
       <rPr>
@@ -51,7 +51,7 @@
     <t>(pk) id_rol</t>
   </si>
   <si>
-    <t>(nn) nombre_rol</t>
+    <t>(nn) rol_name</t>
   </si>
   <si>
     <t>Administrador</t>
@@ -246,7 +246,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> pertenecen muchas </t>
+      <t xml:space="preserve"> pertenece a muchas </t>
     </r>
     <r>
       <rPr>
@@ -382,24 +382,65 @@
     <t>(pk) id_product</t>
   </si>
   <si>
+    <t>(nn) id_suplier</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Un </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Producto</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Contiene un </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Detalle</t>
+    </r>
+  </si>
+  <si>
+    <t>DETALLES</t>
+  </si>
+  <si>
+    <t>(fk) id_product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(pk) product_serial </t>
+  </si>
+  <si>
     <t>(nn) product_name</t>
   </si>
   <si>
-    <t>(nn) product_serial</t>
-  </si>
-  <si>
     <t>(DATE) product_admmision_date</t>
   </si>
   <si>
     <t>(FLOAT) product_price</t>
   </si>
   <si>
+    <t>154-7G3M-92XQ</t>
+  </si>
+  <si>
     <t>Lenovo thinkpad 14´</t>
   </si>
   <si>
-    <t>154-7G3M-92XQ</t>
-  </si>
-  <si>
     <t>154-B4J8-6NWP</t>
   </si>
   <si>
@@ -451,9 +492,6 @@
   </si>
   <si>
     <t>GARANTIAS</t>
-  </si>
-  <si>
-    <t>(fk) id_product</t>
   </si>
   <si>
     <t>(pk) id_warranty</t>
@@ -1336,9 +1374,6 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
     </row>
     <row r="47">
       <c r="B47" s="4" t="s">
@@ -1350,15 +1385,6 @@
       <c r="D47" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="48">
       <c r="B48" s="5">
@@ -1367,18 +1393,10 @@
       <c r="C48" s="5">
         <v>1.0</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F48" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="G48" s="12">
-        <v>500000.0</v>
-      </c>
+      <c r="D48" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H48" s="6"/>
     </row>
     <row r="49">
       <c r="B49" s="5">
@@ -1387,17 +1405,8 @@
       <c r="C49" s="5">
         <v>2.0</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F49" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="G49" s="12">
-        <v>500000.0</v>
+      <c r="D49" s="5">
+        <v>1.0</v>
       </c>
     </row>
     <row r="50">
@@ -1407,17 +1416,8 @@
       <c r="C50" s="5">
         <v>3.0</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F50" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="G50" s="12">
-        <v>500000.0</v>
+      <c r="D50" s="5">
+        <v>1.0</v>
       </c>
     </row>
     <row r="51">
@@ -1427,17 +1427,8 @@
       <c r="C51" s="5">
         <v>4.0</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F51" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="G51" s="12">
-        <v>500000.0</v>
+      <c r="D51" s="5">
+        <v>2.0</v>
       </c>
     </row>
     <row r="52">
@@ -1447,17 +1438,8 @@
       <c r="C52" s="5">
         <v>5.0</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F52" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="G52" s="12">
-        <v>500000.0</v>
+      <c r="D52" s="5">
+        <v>3.0</v>
       </c>
     </row>
     <row r="53">
@@ -1467,17 +1449,8 @@
       <c r="C53" s="5">
         <v>6.0</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F53" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="G53" s="12">
-        <v>500000.0</v>
+      <c r="D53" s="5">
+        <v>4.0</v>
       </c>
     </row>
     <row r="54">
@@ -1487,286 +1460,302 @@
       <c r="C54" s="5">
         <v>7.0</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F54" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="G54" s="12">
-        <v>500000.0</v>
+      <c r="D54" s="5">
+        <v>5.0</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="6" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57">
-      <c r="B57" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
+      <c r="B57" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
     </row>
     <row r="58">
       <c r="B58" s="4" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>82</v>
+        <v>71</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" s="5">
         <v>1.0</v>
       </c>
-      <c r="C59" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D59" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="E59" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>83</v>
+      <c r="C59" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E59" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="F59" s="12">
+        <v>500000.0</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" s="5">
         <v>2.0</v>
       </c>
-      <c r="C60" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="D60" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="E60" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>84</v>
+      <c r="C60" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="F60" s="12">
+        <v>500000.0</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" s="5">
         <v>3.0</v>
       </c>
-      <c r="C61" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="D61" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="E61" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>85</v>
+      <c r="C61" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E61" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="F61" s="12">
+        <v>500000.0</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" s="5">
         <v>4.0</v>
       </c>
-      <c r="C62" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="D62" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="E62" s="5">
-        <v>0.0</v>
+      <c r="C62" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E62" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="F62" s="12">
+        <v>500000.0</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" s="5">
         <v>5.0</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C63" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E63" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="F63" s="12">
+        <v>500000.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E64" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="F64" s="12">
+        <v>500000.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E65" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="F65" s="12">
+        <v>500000.0</v>
+      </c>
+    </row>
+    <row r="67" ht="26.25" customHeight="1">
+      <c r="B67" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" ht="17.25" customHeight="1">
+      <c r="B68" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+    </row>
+    <row r="69">
+      <c r="B69" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C70" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D70" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="E70" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="C71" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D71" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="E71" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="C72" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D72" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="E72" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="C73" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="D73" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" s="5">
         <v>5.0</v>
       </c>
-      <c r="D63" s="11">
-        <v>43866.0</v>
-      </c>
-      <c r="E63" s="5">
+      <c r="C74" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D74" s="11">
+        <v>43866.0</v>
+      </c>
+      <c r="E74" s="5">
         <v>0.0</v>
       </c>
     </row>
-    <row r="65">
-      <c r="B65" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="B66" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-    </row>
-    <row r="67">
-      <c r="B67" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D67" s="4" t="s">
+    <row r="76">
+      <c r="B76" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E67" s="4" t="s">
+    </row>
+    <row r="77">
+      <c r="B77" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="68" ht="42.0" customHeight="1">
-      <c r="B68" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="C68" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="D68" s="9" t="s">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78">
+      <c r="B78" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E68" s="15">
-        <v>43866.0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="B69" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="C69" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E69" s="15">
-        <v>43866.0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="B70" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="C70" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E70" s="15">
-        <v>43866.0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="B71" s="8">
-        <v>4.0</v>
-      </c>
-      <c r="C71" s="8">
-        <v>4.0</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E71" s="15">
-        <v>43866.0</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="B72" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="C72" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E72" s="15">
-        <v>43866.0</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="B74" s="6" t="s">
+      <c r="D78" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="75">
-      <c r="B75" s="2" t="s">
+      <c r="E78" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-    </row>
-    <row r="76">
-      <c r="B76" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="C77" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="D77" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E77" s="15">
-        <v>43866.0</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="C78" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="D78" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E78" s="15">
-        <v>43866.0</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" s="8">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C79" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="D79" s="16" t="s">
-        <v>100</v>
+        <v>1.0</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="E79" s="15">
         <v>43866.0</v>
@@ -1774,13 +1763,13 @@
     </row>
     <row r="80">
       <c r="B80" s="8">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C80" s="8">
-        <v>4.0</v>
-      </c>
-      <c r="D80" s="16" t="s">
-        <v>100</v>
+        <v>2.0</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="E80" s="15">
         <v>43866.0</v>
@@ -1788,15 +1777,140 @@
     </row>
     <row r="81">
       <c r="B81" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="C81" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E81" s="15">
+        <v>43866.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="C82" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E82" s="15">
+        <v>43866.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" s="8">
         <v>5.0</v>
       </c>
-      <c r="C81" s="8">
+      <c r="C83" s="8">
         <v>5.0</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="D83" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E83" s="15">
+        <v>43866.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87">
+      <c r="B87" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E87" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E81" s="15">
+    </row>
+    <row r="88">
+      <c r="B88" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C88" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E88" s="15">
+        <v>43866.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C89" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E89" s="15">
+        <v>43866.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="C90" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="D90" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E90" s="15">
+        <v>43866.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="C91" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E91" s="15">
+        <v>43866.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="C92" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="D92" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E92" s="15">
         <v>43866.0</v>
       </c>
     </row>

</xml_diff>